<commit_message>
stuck on objective function
</commit_message>
<xml_diff>
--- a/ornekgorev.xlsx
+++ b/ornekgorev.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolat\Desktop\mat_koy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolat\Desktop\repos\NMK-daily-work-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CCC995-E6B3-40C2-8427-936CAE8F0297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960BDFFE-62D0-485C-897E-962F9E3C0C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A13E096E-6D95-4C98-B9EF-105EBE77CF77}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>Kahvaltı hazırlığı</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>w_4</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Weights</t>
   </si>
 </sst>
 </file>
@@ -499,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98FCBC65-CC05-4167-A3D0-A969063AA734}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,25 +516,25 @@
     <col min="1" max="1" width="87.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
@@ -536,31 +542,31 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>33</v>
@@ -568,39 +574,39 @@
     </row>
     <row r="8" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>33</v>
@@ -608,39 +614,39 @@
     </row>
     <row r="13" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>33</v>
@@ -648,23 +654,23 @@
     </row>
     <row r="18" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>33</v>
@@ -672,31 +678,31 @@
     </row>
     <row r="21" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>33</v>
@@ -704,39 +710,39 @@
     </row>
     <row r="25" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>31</v>
@@ -744,9 +750,17 @@
     </row>
     <row r="30" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
kullanıcı 1 den büyük her inputu girebilir
</commit_message>
<xml_diff>
--- a/ornekgorev.xlsx
+++ b/ornekgorev.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolat\Desktop\repos\NMK-daily-work-assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolat\Desktop\mat_koy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960BDFFE-62D0-485C-897E-962F9E3C0C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E722EC42-43BE-4815-8C2C-CDB6A69ED6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A13E096E-6D95-4C98-B9EF-105EBE77CF77}"/>
   </bookViews>
@@ -140,10 +140,10 @@
     <t>w_4</t>
   </si>
   <si>
+    <t>Weights</t>
+  </si>
+  <si>
     <t>Tasks</t>
-  </si>
-  <si>
-    <t>Weights</t>
   </si>
 </sst>
 </file>
@@ -189,7 +189,7 @@
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,7 +508,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,10 +518,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
@@ -529,7 +529,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
@@ -537,7 +537,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
@@ -545,7 +545,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
@@ -553,7 +553,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
@@ -585,7 +585,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
@@ -625,7 +625,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
@@ -665,7 +665,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
@@ -729,7 +729,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">

</xml_diff>